<commit_message>
Added our stm32 open ventilator project to the list.
</commit_message>
<xml_diff>
--- a/Covid19_Projects_from_YouTube.xlsx
+++ b/Covid19_Projects_from_YouTube.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertread/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@2018\en.stm32cubef4\STM32Cube_FW_F4_V1.21.0\Projects\STM32F4-Discovery\Examples\UART\covid19-vent-list\covid19-vent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84208DF-AC97-DC4E-A42E-9F4A347FACC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="3240" windowWidth="27580" windowHeight="24140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="3240" windowWidth="27585" windowHeight="24135" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="457">
   <si>
     <t>Project Number</t>
   </si>
@@ -1401,11 +1400,26 @@
   <si>
     <t>Ambu-Bag Mechanism</t>
   </si>
+  <si>
+    <t>STM32 Open Ventilator</t>
+  </si>
+  <si>
+    <t>STM32 Open Ventilator Presentation</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=p47dtsTrSBI</t>
+  </si>
+  <si>
+    <t>https://github.com/STM32OV/OV/blob/master/STM32%20Open%20Ventilator.png</t>
+  </si>
+  <si>
+    <t>STM32 Open Ventilator org</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16">
     <font>
       <sz val="11"/>
@@ -2023,29 +2037,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H129" sqref="H129"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="34" style="2" customWidth="1"/>
-    <col min="9" max="9" width="45.1640625" style="2" customWidth="1"/>
-    <col min="10" max="1025" width="9.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="45.140625" style="2" customWidth="1"/>
+    <col min="10" max="1025" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="40">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="56.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33">
+    <row r="2" spans="1:9" ht="31.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2094,7 +2108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33">
+    <row r="3" spans="1:9" ht="31.5">
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
@@ -2104,7 +2118,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="33">
+    <row r="4" spans="1:9" ht="46.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2132,7 +2146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="10" customFormat="1" ht="33">
+    <row r="6" spans="1:9" s="10" customFormat="1" ht="31.5">
       <c r="A6" s="9"/>
       <c r="E6" s="3" t="s">
         <v>17</v>
@@ -2147,7 +2161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" ht="49">
+    <row r="7" spans="1:9" s="10" customFormat="1" ht="61.5">
       <c r="A7" s="9"/>
       <c r="B7" s="6"/>
       <c r="E7" s="3" t="s">
@@ -2163,7 +2177,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="33">
+    <row r="8" spans="1:9" ht="31.5">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -2183,7 +2197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="33">
+    <row r="9" spans="1:9" ht="31.5">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -2200,7 +2214,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="49">
+    <row r="10" spans="1:9" ht="61.5">
       <c r="G10" s="3" t="s">
         <v>38</v>
       </c>
@@ -2211,7 +2225,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="33">
+    <row r="11" spans="1:9" ht="31.5">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -2228,7 +2242,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="33">
+    <row r="12" spans="1:9" ht="31.5">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -2245,7 +2259,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="33">
+    <row r="13" spans="1:9" ht="31.5">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -2262,7 +2276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="49">
+    <row r="14" spans="1:9" ht="46.5">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -2279,7 +2293,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="33">
+    <row r="15" spans="1:9" ht="31.5">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -2309,7 +2323,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="33">
+    <row r="18" spans="1:9" ht="31.5">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -2326,7 +2340,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="33">
+    <row r="19" spans="1:9" ht="31.5">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -2343,7 +2357,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="33">
+    <row r="20" spans="1:9" ht="31.5">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -2360,7 +2374,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="49">
+    <row r="21" spans="1:9" ht="61.5">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -2383,7 +2397,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="49">
+    <row r="22" spans="1:9" ht="61.5">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -2400,7 +2414,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="49">
+    <row r="23" spans="1:9" ht="76.5">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -2443,19 +2457,19 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="31.5">
       <c r="C28" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G28" s="12"/>
     </row>
-    <row r="29" spans="1:9" ht="33">
+    <row r="29" spans="1:9" ht="31.5">
       <c r="C29" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:9" ht="49">
+    <row r="30" spans="1:9" ht="61.5">
       <c r="A30" s="1">
         <v>16</v>
       </c>
@@ -2472,7 +2486,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="48">
+    <row r="31" spans="1:9" ht="60">
       <c r="E31" s="3" t="s">
         <v>85</v>
       </c>
@@ -2486,7 +2500,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="65">
+    <row r="32" spans="1:9" ht="61.5">
       <c r="A32" s="1">
         <v>18</v>
       </c>
@@ -2503,7 +2517,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="49">
+    <row r="33" spans="1:9" ht="61.5">
       <c r="A33" s="1">
         <v>19</v>
       </c>
@@ -2523,7 +2537,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="49">
+    <row r="34" spans="1:9" ht="61.5">
       <c r="A34" s="1">
         <v>20</v>
       </c>
@@ -2548,7 +2562,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="65">
+    <row r="36" spans="1:9" ht="76.5">
       <c r="A36" s="1">
         <v>21</v>
       </c>
@@ -2568,7 +2582,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="49">
+    <row r="37" spans="1:9" ht="61.5">
       <c r="A37" s="1">
         <v>22</v>
       </c>
@@ -2588,7 +2602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="65">
+    <row r="38" spans="1:9" ht="61.5">
       <c r="A38" s="1">
         <v>23</v>
       </c>
@@ -2613,7 +2627,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="49">
+    <row r="40" spans="1:9" ht="61.5">
       <c r="A40" s="1">
         <v>24</v>
       </c>
@@ -2633,7 +2647,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="49">
+    <row r="41" spans="1:9" ht="61.5">
       <c r="A41" s="1">
         <v>25</v>
       </c>
@@ -2650,7 +2664,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="49">
+    <row r="42" spans="1:9" ht="61.5">
       <c r="A42" s="1">
         <v>26</v>
       </c>
@@ -2667,7 +2681,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="49">
+    <row r="43" spans="1:9" ht="61.5">
       <c r="A43" s="1">
         <v>27</v>
       </c>
@@ -2684,7 +2698,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="49">
+    <row r="44" spans="1:9" ht="61.5">
       <c r="A44" s="1">
         <v>28</v>
       </c>
@@ -2704,7 +2718,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="49">
+    <row r="45" spans="1:9" ht="61.5">
       <c r="A45" s="1">
         <v>29</v>
       </c>
@@ -2724,7 +2738,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="65">
+    <row r="46" spans="1:9" ht="61.5">
       <c r="A46" s="1">
         <v>30</v>
       </c>
@@ -2744,7 +2758,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="49">
+    <row r="47" spans="1:9" ht="61.5">
       <c r="A47" s="1">
         <v>31</v>
       </c>
@@ -2761,7 +2775,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="49">
+    <row r="48" spans="1:9" ht="61.5">
       <c r="A48" s="1">
         <v>32</v>
       </c>
@@ -2783,7 +2797,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="65">
+    <row r="50" spans="1:9" ht="61.5">
       <c r="A50" s="1">
         <v>33</v>
       </c>
@@ -2800,7 +2814,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="49">
+    <row r="51" spans="1:9" ht="61.5">
       <c r="A51" s="1">
         <v>34</v>
       </c>
@@ -2820,7 +2834,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="49">
+    <row r="52" spans="1:9" ht="61.5">
       <c r="A52" s="1">
         <v>35</v>
       </c>
@@ -2837,7 +2851,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="65">
+    <row r="53" spans="1:9" ht="61.5">
       <c r="A53" s="1">
         <v>36</v>
       </c>
@@ -2862,7 +2876,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="49">
+    <row r="55" spans="1:9" ht="61.5">
       <c r="B55" s="10"/>
       <c r="G55" s="3" t="s">
         <v>191</v>
@@ -2874,7 +2888,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="65">
+    <row r="56" spans="1:9" ht="61.5">
       <c r="A56" s="1">
         <v>37</v>
       </c>
@@ -2891,7 +2905,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="49">
+    <row r="57" spans="1:9" ht="61.5">
       <c r="A57" s="1">
         <v>38</v>
       </c>
@@ -2911,7 +2925,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="49">
+    <row r="58" spans="1:9" ht="61.5">
       <c r="A58" s="1">
         <v>39</v>
       </c>
@@ -2937,7 +2951,7 @@
       </c>
       <c r="D59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="65">
+    <row r="60" spans="1:9" ht="61.5">
       <c r="B60" s="10"/>
       <c r="G60" s="3" t="s">
         <v>209</v>
@@ -2949,7 +2963,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="65">
+    <row r="61" spans="1:9" ht="61.5">
       <c r="A61" s="1">
         <v>41</v>
       </c>
@@ -2966,7 +2980,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="49">
+    <row r="62" spans="1:9" ht="61.5">
       <c r="A62" s="1">
         <v>43</v>
       </c>
@@ -2983,7 +2997,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="49">
+    <row r="63" spans="1:9" ht="61.5">
       <c r="A63" s="1">
         <v>44</v>
       </c>
@@ -3003,7 +3017,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="49">
+    <row r="64" spans="1:9" ht="61.5">
       <c r="A64" s="1">
         <v>45</v>
       </c>
@@ -3028,7 +3042,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="49">
+    <row r="66" spans="1:9" ht="61.5">
       <c r="A66" s="1">
         <v>46</v>
       </c>
@@ -3045,7 +3059,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="49">
+    <row r="67" spans="1:9" ht="61.5">
       <c r="A67" s="1">
         <v>47</v>
       </c>
@@ -3065,7 +3079,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="65">
+    <row r="68" spans="1:9" ht="61.5">
       <c r="A68" s="1">
         <v>48</v>
       </c>
@@ -3090,7 +3104,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="49">
+    <row r="70" spans="1:9" ht="61.5">
       <c r="A70" s="1">
         <v>51</v>
       </c>
@@ -3107,7 +3121,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="49">
+    <row r="71" spans="1:9" ht="61.5">
       <c r="A71" s="1">
         <v>53</v>
       </c>
@@ -3130,12 +3144,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="97">
+    <row r="72" spans="1:9" ht="106.5">
       <c r="C72" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="33">
+    <row r="73" spans="1:9" ht="31.5">
       <c r="C73" s="2" t="s">
         <v>257</v>
       </c>
@@ -3160,7 +3174,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="49">
+    <row r="79" spans="1:9" ht="61.5">
       <c r="A79" s="1">
         <v>54</v>
       </c>
@@ -3180,7 +3194,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" ht="31.5">
       <c r="C80" s="2" t="s">
         <v>267</v>
       </c>
@@ -3190,7 +3204,7 @@
       <c r="E81" s="21"/>
       <c r="G81" s="21"/>
     </row>
-    <row r="82" spans="1:9" ht="33">
+    <row r="82" spans="1:9" ht="46.5">
       <c r="A82" s="1">
         <v>55</v>
       </c>
@@ -3214,7 +3228,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="33">
+    <row r="83" spans="1:9" ht="31.5">
       <c r="A83" s="1">
         <v>56</v>
       </c>
@@ -3231,7 +3245,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="33">
+    <row r="84" spans="1:9" ht="31.5">
       <c r="A84" s="1">
         <v>57</v>
       </c>
@@ -3254,12 +3268,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="81">
+    <row r="85" spans="1:9" ht="106.5">
       <c r="C85" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="33">
+    <row r="86" spans="1:9" ht="31.5">
       <c r="A86" s="1">
         <v>58</v>
       </c>
@@ -3276,7 +3290,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="65">
+    <row r="87" spans="1:9" ht="61.5">
       <c r="A87" s="1">
         <v>59</v>
       </c>
@@ -3296,19 +3310,19 @@
         <v>293</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="33">
+    <row r="88" spans="1:9" ht="31.5">
       <c r="H88" s="8"/>
       <c r="I88" s="6" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="33">
+    <row r="89" spans="1:9" ht="31.5">
       <c r="H89" s="8"/>
       <c r="I89" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="33">
+    <row r="90" spans="1:9" ht="31.5">
       <c r="A90" s="1">
         <v>60</v>
       </c>
@@ -3325,7 +3339,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="33">
+    <row r="91" spans="1:9" ht="31.5">
       <c r="A91" s="1">
         <v>61</v>
       </c>
@@ -3342,7 +3356,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="33">
+    <row r="92" spans="1:9" ht="46.5">
       <c r="A92" s="1">
         <v>62</v>
       </c>
@@ -3365,7 +3379,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="33">
+    <row r="93" spans="1:9" ht="31.5">
       <c r="B93" s="2" t="s">
         <v>309</v>
       </c>
@@ -3373,7 +3387,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="33">
+    <row r="94" spans="1:9" ht="31.5">
       <c r="A94" s="1">
         <v>63</v>
       </c>
@@ -3390,7 +3404,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" ht="31.5">
       <c r="A95" s="1">
         <v>64</v>
       </c>
@@ -3407,7 +3421,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="33">
+    <row r="96" spans="1:9" ht="31.5">
       <c r="G96" s="3" t="s">
         <v>319</v>
       </c>
@@ -3418,7 +3432,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="33">
+    <row r="97" spans="1:9" ht="31.5">
       <c r="A97" s="1">
         <v>65</v>
       </c>
@@ -3438,7 +3452,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="33">
+    <row r="98" spans="1:9" ht="31.5">
       <c r="A98" s="1">
         <v>66</v>
       </c>
@@ -3458,7 +3472,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="33">
+    <row r="99" spans="1:9" ht="31.5">
       <c r="A99" s="1">
         <v>67</v>
       </c>
@@ -3478,7 +3492,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="33">
+    <row r="100" spans="1:9" ht="31.5">
       <c r="B100" s="2" t="s">
         <v>337</v>
       </c>
@@ -3499,7 +3513,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="33">
+    <row r="101" spans="1:9" ht="31.5">
       <c r="A101" s="1">
         <v>68</v>
       </c>
@@ -3516,7 +3530,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="2" customFormat="1" ht="33">
+    <row r="102" spans="1:9" s="2" customFormat="1" ht="31.5">
       <c r="A102" s="1">
         <v>69</v>
       </c>
@@ -3530,7 +3544,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="113">
+    <row r="103" spans="1:9" ht="121.5">
       <c r="A103" s="1">
         <v>70</v>
       </c>
@@ -3550,12 +3564,12 @@
         <v>351</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="145">
+    <row r="104" spans="1:9" ht="151.5">
       <c r="C104" s="6" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="33">
+    <row r="105" spans="1:9" ht="31.5">
       <c r="A105" s="1">
         <v>71</v>
       </c>
@@ -3572,7 +3586,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="33">
+    <row r="106" spans="1:9" ht="31.5">
       <c r="A106" s="1">
         <v>72</v>
       </c>
@@ -3589,7 +3603,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="33">
+    <row r="107" spans="1:9" ht="31.5">
       <c r="G107" s="3" t="s">
         <v>360</v>
       </c>
@@ -3600,7 +3614,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="33">
+    <row r="108" spans="1:9" ht="31.5">
       <c r="A108" s="1">
         <v>73</v>
       </c>
@@ -3617,7 +3631,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="33">
+    <row r="109" spans="1:9" ht="31.5">
       <c r="A109" s="1">
         <v>74</v>
       </c>
@@ -3634,7 +3648,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="33">
+    <row r="110" spans="1:9" ht="31.5">
       <c r="A110" s="1">
         <v>75</v>
       </c>
@@ -3657,19 +3671,19 @@
         <v>376</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="33">
+    <row r="111" spans="1:9" ht="31.5">
       <c r="H111" s="8"/>
       <c r="I111" s="6" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="33">
+    <row r="112" spans="1:9" ht="31.5">
       <c r="H112" s="8"/>
       <c r="I112" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="33">
+    <row r="113" spans="1:10" ht="31.5">
       <c r="A113" s="1">
         <v>76</v>
       </c>
@@ -3689,7 +3703,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="33">
+    <row r="114" spans="1:10" ht="31.5">
       <c r="G114" s="3" t="s">
         <v>384</v>
       </c>
@@ -3700,7 +3714,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="33">
+    <row r="115" spans="1:10" ht="31.5">
       <c r="A115" s="1">
         <v>77</v>
       </c>
@@ -3717,7 +3731,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="33">
+    <row r="116" spans="1:10" ht="31.5">
       <c r="A116" s="1">
         <v>78</v>
       </c>
@@ -3737,7 +3751,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="33">
+    <row r="117" spans="1:10" ht="31.5">
       <c r="A117" s="1">
         <v>79</v>
       </c>
@@ -3762,7 +3776,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="97">
+    <row r="119" spans="1:10" ht="106.5">
       <c r="A119" s="1">
         <v>80</v>
       </c>
@@ -3793,7 +3807,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="113">
+    <row r="121" spans="1:10" ht="121.5">
       <c r="A121" s="1">
         <v>81</v>
       </c>
@@ -3813,7 +3827,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="33">
+    <row r="122" spans="1:10" ht="31.5">
       <c r="A122" s="1">
         <v>82</v>
       </c>
@@ -3836,7 +3850,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="33">
+    <row r="123" spans="1:10" ht="31.5">
       <c r="A123" s="1">
         <v>83</v>
       </c>
@@ -3853,7 +3867,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="33">
+    <row r="124" spans="1:10" ht="46.5">
       <c r="A124" s="1">
         <v>84</v>
       </c>
@@ -3881,7 +3895,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="129">
+    <row r="126" spans="1:10" ht="136.5">
       <c r="A126" s="1">
         <v>85</v>
       </c>
@@ -3901,7 +3915,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="32">
+    <row r="127" spans="1:10" ht="30">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -3915,7 +3929,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="97">
+    <row r="128" spans="1:10" ht="91.5">
       <c r="A128" s="1">
         <v>86</v>
       </c>
@@ -3938,7 +3952,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="129" spans="2:8">
+    <row r="129" spans="2:9">
       <c r="B129" s="29" t="s">
         <v>451</v>
       </c>
@@ -3958,245 +3972,264 @@
         <v>447</v>
       </c>
     </row>
-    <row r="131" spans="2:8" ht="33">
+    <row r="130" spans="2:9" ht="31.5">
+      <c r="D130" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="H130" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="I130" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" ht="46.5">
       <c r="B131" s="2" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="132" spans="2:8">
+    <row r="132" spans="2:9" ht="31.5">
       <c r="B132" s="6" t="s">
         <v>446</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="I5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="I8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="I9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="H11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="I11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="H12" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="I12" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="H13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H14" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="I14" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="H15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I15" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="H18" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="H19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="I19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="H20" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="I20" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C21" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H21" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="I21" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H22" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="I22" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="H23" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="I23" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C26" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H30" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H31" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="H32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="I32" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="H33" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="I33" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="H34" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="I34" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C36" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="H36" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="I36" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C37" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="H37" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="I37" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="H38" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="I38" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C40" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="H40" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="I40" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="H41" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="I41" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="H42" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="I42" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="H43" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="I43" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="H44" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="I44" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="H45" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="I45" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C46" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="H46" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="I46" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="H47" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="I47" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="H48" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="I48" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="H50" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="I50" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="H51" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="I51" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="H52" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="I52" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="H53" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="I53" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C54" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="H55" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="H56" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="H57" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="I57" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="H58" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="I58" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="H60" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="I60" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="H61" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="I61" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="H62" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="I62" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C63" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="H63" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="I63" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="H64" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="I64" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="H66" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="I66" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="H67" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="I67" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="H68" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="I68" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="H70" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="I70" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="H71" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="I71" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="H79" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="I79" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="H82" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="I82" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="E83" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="H83" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="I83" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="E84" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="H84" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="I84" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="E86" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="H86" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="I86" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="E87" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="H87" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="I87" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="I88" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="I89" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="E90" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="H90" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="I90" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="E91" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="H91" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="I91" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="E92" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="H92" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="I92" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="E94" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="H94" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="I94" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="E95" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="H95" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="H96" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="I96" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="E97" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="H97" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="E98" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="H98" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="I98" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="C99" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="E99" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="H99" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="I99" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="D100" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="H100" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="I100" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="E101" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="H101" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="I101" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="H102" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="I102" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="C103" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="E103" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="H103" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="I103" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="C104" r:id="rId164" display="https://www.youtube.com/redirect?q=https%3A%2F%2Fhackaday.com%2F2020%2F03%2F12%2Fultimate-medical-hackathon-how-fast-can-we-design-and-deploy-an-open-source-ventilator&amp;redir_token=Sn1b0sNvlpxXEVmr4n3vpumPwxt8MTU4NTY4NzA4NUAxNTg1NjAwNjg1&amp;v=zawkJRm_7aI&amp;event=video_description" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="E105" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="H105" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="I105" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="E106" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="H106" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="I106" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="H107" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="I107" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="E108" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="H108" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="I108" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="E109" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="H109" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="I109" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="E110" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="H110" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="I110" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="I111" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="I112" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="E113" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="H113" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="I113" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="H114" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="I114" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="E115" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="H115" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="I115" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="E116" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="H116" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="I116" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="C117" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="E117" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="H117" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="I117" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="C119" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="E119" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="H119" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="I119" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="C120" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="C121" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="E121" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="H121" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="I121" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="E122" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="H122" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="I122" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="E123" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="H123" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="I123" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="E124" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="H124" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="I124" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="C126" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="E126" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="H126" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="I126" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="H127" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="I127" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="H128" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="J128" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="B132" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="C129" r:id="rId226" display="https://www.youtube.com/watch?v=ES7VPJ-tg3k&amp;feature=youtu.be" xr:uid="{BFF22F32-2E88-BF4F-9A4E-9248AEFEAE6D}"/>
-    <hyperlink ref="H129" r:id="rId227" xr:uid="{8DFF2B1F-0901-D041-8EA5-FCD37E4AD651}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="I5" r:id="rId7"/>
+    <hyperlink ref="H6" r:id="rId8"/>
+    <hyperlink ref="H7" r:id="rId9"/>
+    <hyperlink ref="H8" r:id="rId10"/>
+    <hyperlink ref="I8" r:id="rId11"/>
+    <hyperlink ref="H9" r:id="rId12"/>
+    <hyperlink ref="I9" r:id="rId13"/>
+    <hyperlink ref="I10" r:id="rId14"/>
+    <hyperlink ref="H11" r:id="rId15"/>
+    <hyperlink ref="I11" r:id="rId16"/>
+    <hyperlink ref="H12" r:id="rId17"/>
+    <hyperlink ref="I12" r:id="rId18"/>
+    <hyperlink ref="H13" r:id="rId19"/>
+    <hyperlink ref="H14" r:id="rId20"/>
+    <hyperlink ref="I14" r:id="rId21"/>
+    <hyperlink ref="H15" r:id="rId22"/>
+    <hyperlink ref="I15" r:id="rId23"/>
+    <hyperlink ref="H18" r:id="rId24"/>
+    <hyperlink ref="H19" r:id="rId25"/>
+    <hyperlink ref="I19" r:id="rId26"/>
+    <hyperlink ref="H20" r:id="rId27"/>
+    <hyperlink ref="I20" r:id="rId28"/>
+    <hyperlink ref="C21" r:id="rId29"/>
+    <hyperlink ref="H21" r:id="rId30"/>
+    <hyperlink ref="I21" r:id="rId31"/>
+    <hyperlink ref="H22" r:id="rId32"/>
+    <hyperlink ref="I22" r:id="rId33"/>
+    <hyperlink ref="H23" r:id="rId34"/>
+    <hyperlink ref="I23" r:id="rId35"/>
+    <hyperlink ref="C26" r:id="rId36"/>
+    <hyperlink ref="H30" r:id="rId37"/>
+    <hyperlink ref="H31" r:id="rId38"/>
+    <hyperlink ref="H32" r:id="rId39"/>
+    <hyperlink ref="I32" r:id="rId40"/>
+    <hyperlink ref="H33" r:id="rId41"/>
+    <hyperlink ref="I33" r:id="rId42"/>
+    <hyperlink ref="H34" r:id="rId43"/>
+    <hyperlink ref="I34" r:id="rId44"/>
+    <hyperlink ref="C36" r:id="rId45"/>
+    <hyperlink ref="H36" r:id="rId46"/>
+    <hyperlink ref="I36" r:id="rId47"/>
+    <hyperlink ref="C37" r:id="rId48"/>
+    <hyperlink ref="H37" r:id="rId49"/>
+    <hyperlink ref="I37" r:id="rId50"/>
+    <hyperlink ref="H38" r:id="rId51"/>
+    <hyperlink ref="I38" r:id="rId52"/>
+    <hyperlink ref="C40" r:id="rId53"/>
+    <hyperlink ref="H40" r:id="rId54"/>
+    <hyperlink ref="I40" r:id="rId55"/>
+    <hyperlink ref="H41" r:id="rId56"/>
+    <hyperlink ref="I41" r:id="rId57"/>
+    <hyperlink ref="H42" r:id="rId58"/>
+    <hyperlink ref="I42" r:id="rId59"/>
+    <hyperlink ref="H43" r:id="rId60"/>
+    <hyperlink ref="I43" r:id="rId61"/>
+    <hyperlink ref="H44" r:id="rId62"/>
+    <hyperlink ref="I44" r:id="rId63"/>
+    <hyperlink ref="H45" r:id="rId64"/>
+    <hyperlink ref="I45" r:id="rId65"/>
+    <hyperlink ref="C46" r:id="rId66"/>
+    <hyperlink ref="H46" r:id="rId67"/>
+    <hyperlink ref="I46" r:id="rId68"/>
+    <hyperlink ref="H47" r:id="rId69"/>
+    <hyperlink ref="I47" r:id="rId70"/>
+    <hyperlink ref="H48" r:id="rId71"/>
+    <hyperlink ref="I48" r:id="rId72"/>
+    <hyperlink ref="H50" r:id="rId73"/>
+    <hyperlink ref="I50" r:id="rId74"/>
+    <hyperlink ref="H51" r:id="rId75"/>
+    <hyperlink ref="I51" r:id="rId76"/>
+    <hyperlink ref="H52" r:id="rId77"/>
+    <hyperlink ref="I52" r:id="rId78"/>
+    <hyperlink ref="H53" r:id="rId79"/>
+    <hyperlink ref="I53" r:id="rId80"/>
+    <hyperlink ref="C54" r:id="rId81"/>
+    <hyperlink ref="H55" r:id="rId82"/>
+    <hyperlink ref="H56" r:id="rId83"/>
+    <hyperlink ref="H57" r:id="rId84"/>
+    <hyperlink ref="I57" r:id="rId85"/>
+    <hyperlink ref="H58" r:id="rId86"/>
+    <hyperlink ref="I58" r:id="rId87"/>
+    <hyperlink ref="H60" r:id="rId88"/>
+    <hyperlink ref="I60" r:id="rId89"/>
+    <hyperlink ref="H61" r:id="rId90"/>
+    <hyperlink ref="I61" r:id="rId91"/>
+    <hyperlink ref="H62" r:id="rId92"/>
+    <hyperlink ref="I62" r:id="rId93"/>
+    <hyperlink ref="C63" r:id="rId94"/>
+    <hyperlink ref="H63" r:id="rId95"/>
+    <hyperlink ref="I63" r:id="rId96"/>
+    <hyperlink ref="H64" r:id="rId97"/>
+    <hyperlink ref="I64" r:id="rId98"/>
+    <hyperlink ref="H66" r:id="rId99"/>
+    <hyperlink ref="I66" r:id="rId100"/>
+    <hyperlink ref="H67" r:id="rId101"/>
+    <hyperlink ref="I67" r:id="rId102"/>
+    <hyperlink ref="H68" r:id="rId103"/>
+    <hyperlink ref="I68" r:id="rId104"/>
+    <hyperlink ref="H70" r:id="rId105"/>
+    <hyperlink ref="I70" r:id="rId106"/>
+    <hyperlink ref="H71" r:id="rId107"/>
+    <hyperlink ref="I71" r:id="rId108"/>
+    <hyperlink ref="H79" r:id="rId109"/>
+    <hyperlink ref="I79" r:id="rId110"/>
+    <hyperlink ref="H82" r:id="rId111"/>
+    <hyperlink ref="I82" r:id="rId112"/>
+    <hyperlink ref="E83" r:id="rId113"/>
+    <hyperlink ref="H83" r:id="rId114"/>
+    <hyperlink ref="I83" r:id="rId115"/>
+    <hyperlink ref="E84" r:id="rId116"/>
+    <hyperlink ref="H84" r:id="rId117"/>
+    <hyperlink ref="I84" r:id="rId118"/>
+    <hyperlink ref="E86" r:id="rId119"/>
+    <hyperlink ref="H86" r:id="rId120"/>
+    <hyperlink ref="I86" r:id="rId121"/>
+    <hyperlink ref="E87" r:id="rId122"/>
+    <hyperlink ref="H87" r:id="rId123"/>
+    <hyperlink ref="I87" r:id="rId124"/>
+    <hyperlink ref="I88" r:id="rId125"/>
+    <hyperlink ref="I89" r:id="rId126"/>
+    <hyperlink ref="E90" r:id="rId127"/>
+    <hyperlink ref="H90" r:id="rId128"/>
+    <hyperlink ref="I90" r:id="rId129"/>
+    <hyperlink ref="E91" r:id="rId130"/>
+    <hyperlink ref="H91" r:id="rId131"/>
+    <hyperlink ref="I91" r:id="rId132"/>
+    <hyperlink ref="E92" r:id="rId133"/>
+    <hyperlink ref="H92" r:id="rId134"/>
+    <hyperlink ref="I92" r:id="rId135"/>
+    <hyperlink ref="E94" r:id="rId136"/>
+    <hyperlink ref="H94" r:id="rId137"/>
+    <hyperlink ref="I94" r:id="rId138"/>
+    <hyperlink ref="E95" r:id="rId139"/>
+    <hyperlink ref="H95" r:id="rId140"/>
+    <hyperlink ref="H96" r:id="rId141"/>
+    <hyperlink ref="I96" r:id="rId142"/>
+    <hyperlink ref="E97" r:id="rId143"/>
+    <hyperlink ref="H97" r:id="rId144"/>
+    <hyperlink ref="E98" r:id="rId145"/>
+    <hyperlink ref="H98" r:id="rId146"/>
+    <hyperlink ref="I98" r:id="rId147"/>
+    <hyperlink ref="C99" r:id="rId148"/>
+    <hyperlink ref="E99" r:id="rId149"/>
+    <hyperlink ref="H99" r:id="rId150"/>
+    <hyperlink ref="I99" r:id="rId151"/>
+    <hyperlink ref="D100" r:id="rId152"/>
+    <hyperlink ref="H100" r:id="rId153"/>
+    <hyperlink ref="I100" r:id="rId154"/>
+    <hyperlink ref="E101" r:id="rId155"/>
+    <hyperlink ref="H101" r:id="rId156"/>
+    <hyperlink ref="I101" r:id="rId157"/>
+    <hyperlink ref="H102" r:id="rId158"/>
+    <hyperlink ref="I102" r:id="rId159"/>
+    <hyperlink ref="C103" r:id="rId160"/>
+    <hyperlink ref="E103" r:id="rId161"/>
+    <hyperlink ref="H103" r:id="rId162"/>
+    <hyperlink ref="I103" r:id="rId163"/>
+    <hyperlink ref="C104" r:id="rId164" display="https://www.youtube.com/redirect?q=https%3A%2F%2Fhackaday.com%2F2020%2F03%2F12%2Fultimate-medical-hackathon-how-fast-can-we-design-and-deploy-an-open-source-ventilator&amp;redir_token=Sn1b0sNvlpxXEVmr4n3vpumPwxt8MTU4NTY4NzA4NUAxNTg1NjAwNjg1&amp;v=zawkJRm_7aI&amp;event=video_description"/>
+    <hyperlink ref="E105" r:id="rId165"/>
+    <hyperlink ref="H105" r:id="rId166"/>
+    <hyperlink ref="I105" r:id="rId167"/>
+    <hyperlink ref="E106" r:id="rId168"/>
+    <hyperlink ref="H106" r:id="rId169"/>
+    <hyperlink ref="I106" r:id="rId170"/>
+    <hyperlink ref="H107" r:id="rId171"/>
+    <hyperlink ref="I107" r:id="rId172"/>
+    <hyperlink ref="E108" r:id="rId173"/>
+    <hyperlink ref="H108" r:id="rId174"/>
+    <hyperlink ref="I108" r:id="rId175"/>
+    <hyperlink ref="E109" r:id="rId176"/>
+    <hyperlink ref="H109" r:id="rId177"/>
+    <hyperlink ref="I109" r:id="rId178"/>
+    <hyperlink ref="E110" r:id="rId179"/>
+    <hyperlink ref="H110" r:id="rId180"/>
+    <hyperlink ref="I110" r:id="rId181"/>
+    <hyperlink ref="I111" r:id="rId182"/>
+    <hyperlink ref="I112" r:id="rId183"/>
+    <hyperlink ref="E113" r:id="rId184"/>
+    <hyperlink ref="H113" r:id="rId185"/>
+    <hyperlink ref="I113" r:id="rId186"/>
+    <hyperlink ref="H114" r:id="rId187"/>
+    <hyperlink ref="I114" r:id="rId188"/>
+    <hyperlink ref="E115" r:id="rId189"/>
+    <hyperlink ref="H115" r:id="rId190"/>
+    <hyperlink ref="I115" r:id="rId191"/>
+    <hyperlink ref="E116" r:id="rId192"/>
+    <hyperlink ref="H116" r:id="rId193"/>
+    <hyperlink ref="I116" r:id="rId194"/>
+    <hyperlink ref="C117" r:id="rId195"/>
+    <hyperlink ref="E117" r:id="rId196"/>
+    <hyperlink ref="H117" r:id="rId197"/>
+    <hyperlink ref="I117" r:id="rId198"/>
+    <hyperlink ref="C119" r:id="rId199"/>
+    <hyperlink ref="E119" r:id="rId200"/>
+    <hyperlink ref="H119" r:id="rId201"/>
+    <hyperlink ref="I119" r:id="rId202"/>
+    <hyperlink ref="C120" r:id="rId203"/>
+    <hyperlink ref="C121" r:id="rId204"/>
+    <hyperlink ref="E121" r:id="rId205"/>
+    <hyperlink ref="H121" r:id="rId206"/>
+    <hyperlink ref="I121" r:id="rId207"/>
+    <hyperlink ref="E122" r:id="rId208"/>
+    <hyperlink ref="H122" r:id="rId209"/>
+    <hyperlink ref="I122" r:id="rId210"/>
+    <hyperlink ref="E123" r:id="rId211"/>
+    <hyperlink ref="H123" r:id="rId212"/>
+    <hyperlink ref="I123" r:id="rId213"/>
+    <hyperlink ref="E124" r:id="rId214"/>
+    <hyperlink ref="H124" r:id="rId215"/>
+    <hyperlink ref="I124" r:id="rId216"/>
+    <hyperlink ref="C126" r:id="rId217"/>
+    <hyperlink ref="E126" r:id="rId218"/>
+    <hyperlink ref="H126" r:id="rId219"/>
+    <hyperlink ref="I126" r:id="rId220"/>
+    <hyperlink ref="H127" r:id="rId221"/>
+    <hyperlink ref="I127" r:id="rId222"/>
+    <hyperlink ref="H128" r:id="rId223"/>
+    <hyperlink ref="J128" r:id="rId224"/>
+    <hyperlink ref="B132" r:id="rId225"/>
+    <hyperlink ref="C129" r:id="rId226" display="https://www.youtube.com/watch?v=ES7VPJ-tg3k&amp;feature=youtu.be"/>
+    <hyperlink ref="H129" r:id="rId227"/>
+    <hyperlink ref="H130" r:id="rId228"/>
+    <hyperlink ref="I130" r:id="rId229"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>